<commit_message>
updates for fixes to digital asset model
</commit_message>
<xml_diff>
--- a/jcp-v4/99-exceldmd/DAM OOTB Data Model.xlsx
+++ b/jcp-v4/99-exceldmd/DAM OOTB Data Model.xlsx
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2604" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2759" uniqueCount="387">
   <si>
     <t>ACTION</t>
   </si>
@@ -1227,6 +1227,66 @@
   <si>
     <t>DISPLAY SEQUENCE</t>
   </si>
+  <si>
+    <t>exifmodel</t>
+  </si>
+  <si>
+    <t>exifpadding</t>
+  </si>
+  <si>
+    <t>1 to 5</t>
+  </si>
+  <si>
+    <t>property_objectkey</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>property_user</t>
+  </si>
+  <si>
+    <t>property_type</t>
+  </si>
+  <si>
+    <t>property_ownershipdata</t>
+  </si>
+  <si>
+    <t>property_originalfilename</t>
+  </si>
+  <si>
+    <t>property_role</t>
+  </si>
+  <si>
+    <t>property_fullobjectpath</t>
+  </si>
+  <si>
+    <t>property_filename</t>
+  </si>
+  <si>
+    <t>File Name Property</t>
+  </si>
+  <si>
+    <t>Full Object Path Property</t>
+  </si>
+  <si>
+    <t>Original File Name Property</t>
+  </si>
+  <si>
+    <t>Role Property</t>
+  </si>
+  <si>
+    <t>Owner Property</t>
+  </si>
+  <si>
+    <t>Type Property</t>
+  </si>
+  <si>
+    <t>User Property</t>
+  </si>
+  <si>
+    <t>Object Key Property</t>
+  </si>
 </sst>
 </file>
 
@@ -1513,7 +1573,307 @@
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2234,11 +2594,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:XEU126"/>
+  <dimension ref="A1:XEU134"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B127" sqref="B127:B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2442,7 +2802,7 @@
         <v>231</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5" s="37" t="s">
@@ -2476,7 +2836,7 @@
         <v>232</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="37" t="s">
@@ -2624,7 +2984,9 @@
       <c r="G10" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="38"/>
+      <c r="H10" s="38" t="s">
+        <v>369</v>
+      </c>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
@@ -2646,7 +3008,7 @@
         <v>268</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="37" t="s">
@@ -2665,10 +3027,18 @@
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
+      <c r="O11" s="25">
+        <v>0</v>
+      </c>
+      <c r="P11" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q11" s="25">
+        <v>100</v>
+      </c>
+      <c r="R11" s="25" t="s">
+        <v>200</v>
+      </c>
       <c r="S11" s="25"/>
       <c r="T11" s="25"/>
       <c r="U11" s="25"/>
@@ -2682,7 +3052,7 @@
       <c r="C12" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="37" t="s">
         <v>217</v>
       </c>
@@ -3192,7 +3562,7 @@
         <v>220</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27" s="36" t="s">
@@ -3202,7 +3572,7 @@
         <v>88</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="H27" s="38"/>
       <c r="I27" s="25"/>
@@ -3226,7 +3596,7 @@
         <v>221</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="36" t="s">
@@ -3236,7 +3606,7 @@
         <v>165</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="H28" s="38"/>
       <c r="I28" s="25"/>
@@ -3260,7 +3630,7 @@
         <v>222</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="36" t="s">
@@ -3270,7 +3640,7 @@
         <v>96</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="H29" s="38"/>
       <c r="I29" s="25"/>
@@ -3294,7 +3664,7 @@
         <v>223</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="36" t="s">
@@ -3304,7 +3674,7 @@
         <v>167</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="H30" s="38"/>
       <c r="I30" s="25"/>
@@ -3328,7 +3698,7 @@
         <v>224</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="36" t="s">
@@ -3338,7 +3708,7 @@
         <v>168</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="H31" s="38"/>
       <c r="I31" s="25"/>
@@ -3362,7 +3732,7 @@
         <v>225</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="36" t="s">
@@ -3464,7 +3834,7 @@
         <v>351</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="36" t="s">
@@ -3498,7 +3868,7 @@
         <v>240</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="36" t="s">
@@ -3532,7 +3902,7 @@
         <v>241</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="36" t="s">
@@ -3563,12 +3933,12 @@
     <row r="38" spans="1:16375" x14ac:dyDescent="0.2">
       <c r="A38" s="36"/>
       <c r="B38" s="36" t="s">
-        <v>326</v>
+        <v>367</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D38" s="36"/>
+      <c r="D38" s="25"/>
       <c r="E38" s="36" t="s">
         <v>285</v>
       </c>
@@ -3597,12 +3967,12 @@
     <row r="39" spans="1:16375" x14ac:dyDescent="0.2">
       <c r="A39" s="36"/>
       <c r="B39" s="36" t="s">
-        <v>327</v>
+        <v>368</v>
       </c>
       <c r="C39" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="36"/>
+      <c r="D39" s="25"/>
       <c r="E39" s="36" t="s">
         <v>285</v>
       </c>
@@ -19987,7 +20357,7 @@
         <v>83</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="36" t="s">
@@ -52761,7 +53131,7 @@
         <v>269</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D42" s="25"/>
       <c r="E42" s="36" t="s">
@@ -52795,7 +53165,7 @@
         <v>270</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="D43" s="25"/>
       <c r="E43" s="36" t="s">
@@ -52863,17 +53233,17 @@
         <v>255</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="D45" s="36"/>
+        <v>162</v>
+      </c>
+      <c r="D45" s="25"/>
       <c r="E45" s="36" t="s">
         <v>314</v>
       </c>
       <c r="F45" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="G45" s="36" t="s">
-        <v>171</v>
+      <c r="G45" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="H45" s="38"/>
       <c r="I45" s="25"/>
@@ -52897,17 +53267,17 @@
         <v>256</v>
       </c>
       <c r="C46" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="D46" s="36"/>
+        <v>31</v>
+      </c>
+      <c r="D46" s="25"/>
       <c r="E46" s="36" t="s">
         <v>314</v>
       </c>
       <c r="F46" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="G46" s="36" t="s">
-        <v>171</v>
+      <c r="G46" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="H46" s="38"/>
       <c r="I46" s="25"/>
@@ -52931,17 +53301,17 @@
         <v>257</v>
       </c>
       <c r="C47" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="D47" s="36"/>
+        <v>162</v>
+      </c>
+      <c r="D47" s="25"/>
       <c r="E47" s="36" t="s">
         <v>314</v>
       </c>
       <c r="F47" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="G47" s="36" t="s">
-        <v>171</v>
+      <c r="G47" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="H47" s="38"/>
       <c r="I47" s="25"/>
@@ -52967,7 +53337,7 @@
       <c r="C48" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="36"/>
+      <c r="D48" s="25"/>
       <c r="E48" s="36" t="s">
         <v>315</v>
       </c>
@@ -52999,9 +53369,9 @@
         <v>242</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="D49" s="36"/>
+        <v>31</v>
+      </c>
+      <c r="D49" s="25"/>
       <c r="E49" s="36" t="s">
         <v>315</v>
       </c>
@@ -53033,7 +53403,7 @@
         <v>352</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>162</v>
+        <v>31</v>
       </c>
       <c r="D50" s="25"/>
       <c r="E50" s="36" t="s">
@@ -53169,7 +53539,7 @@
         <v>253</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="D54" s="25"/>
       <c r="E54" s="36" t="s">
@@ -53203,7 +53573,7 @@
         <v>161</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>162</v>
+        <v>31</v>
       </c>
       <c r="D55" s="25"/>
       <c r="E55" s="36" t="s">
@@ -53305,7 +53675,7 @@
         <v>276</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="D58" s="25"/>
       <c r="E58" s="36" t="s">
@@ -53339,7 +53709,7 @@
         <v>328</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="D59" s="25"/>
       <c r="E59" s="36" t="s">
@@ -53407,7 +53777,7 @@
         <v>264</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D61" s="25"/>
       <c r="E61" s="36" t="s">
@@ -53475,7 +53845,7 @@
         <v>86</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="D63" s="25"/>
       <c r="E63" s="36" t="s">
@@ -53815,7 +54185,7 @@
         <v>278</v>
       </c>
       <c r="C73" s="25" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="D73" s="25"/>
       <c r="E73" s="36" t="s">
@@ -53951,7 +54321,7 @@
         <v>218</v>
       </c>
       <c r="C77" s="25" t="s">
-        <v>162</v>
+        <v>31</v>
       </c>
       <c r="D77" s="25"/>
       <c r="E77" s="36" t="s">
@@ -54087,7 +54457,7 @@
         <v>250</v>
       </c>
       <c r="C81" s="25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D81" s="25"/>
       <c r="E81" s="36" t="s">
@@ -54121,7 +54491,7 @@
         <v>251</v>
       </c>
       <c r="C82" s="25" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="D82" s="25"/>
       <c r="E82" s="36" t="s">
@@ -54198,7 +54568,7 @@
       <c r="F84" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="G84" s="36" t="s">
+      <c r="G84" s="25" t="s">
         <v>171</v>
       </c>
       <c r="H84" s="39"/>
@@ -54232,7 +54602,7 @@
       <c r="F85" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="G85" s="36" t="s">
+      <c r="G85" s="25" t="s">
         <v>171</v>
       </c>
       <c r="H85" s="38"/>
@@ -54257,7 +54627,7 @@
         <v>233</v>
       </c>
       <c r="C86" s="25" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D86" s="25"/>
       <c r="E86" s="36" t="s">
@@ -54267,7 +54637,7 @@
         <v>172</v>
       </c>
       <c r="G86" s="25" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="H86" s="38"/>
       <c r="I86" s="25"/>
@@ -54291,7 +54661,7 @@
         <v>235</v>
       </c>
       <c r="C87" s="25" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D87" s="25"/>
       <c r="E87" s="36" t="s">
@@ -54301,7 +54671,7 @@
         <v>170</v>
       </c>
       <c r="G87" s="25" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="H87" s="38"/>
       <c r="I87" s="25"/>
@@ -54395,7 +54765,7 @@
       <c r="C90" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D90" s="36"/>
+      <c r="D90" s="25"/>
       <c r="E90" s="36" t="s">
         <v>313</v>
       </c>
@@ -54427,7 +54797,7 @@
         <v>203</v>
       </c>
       <c r="C91" s="25" t="s">
-        <v>31</v>
+        <v>171</v>
       </c>
       <c r="D91" s="25"/>
       <c r="E91" s="36" t="s">
@@ -54437,7 +54807,7 @@
         <v>291</v>
       </c>
       <c r="G91" s="25" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="H91" s="38"/>
       <c r="I91" s="25"/>
@@ -54461,7 +54831,7 @@
         <v>203</v>
       </c>
       <c r="C92" s="25" t="s">
-        <v>31</v>
+        <v>171</v>
       </c>
       <c r="D92" s="25"/>
       <c r="E92" s="36" t="s">
@@ -54471,7 +54841,7 @@
         <v>208</v>
       </c>
       <c r="G92" s="25" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="H92" s="38"/>
       <c r="I92" s="25"/>
@@ -54495,7 +54865,7 @@
         <v>204</v>
       </c>
       <c r="C93" s="25" t="s">
-        <v>31</v>
+        <v>171</v>
       </c>
       <c r="D93" s="25"/>
       <c r="E93" s="36" t="s">
@@ -54505,7 +54875,7 @@
         <v>209</v>
       </c>
       <c r="G93" s="25" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="H93" s="38"/>
       <c r="I93" s="25"/>
@@ -54538,7 +54908,7 @@
       <c r="F94" s="36" t="s">
         <v>292</v>
       </c>
-      <c r="G94" s="36" t="s">
+      <c r="G94" s="25" t="s">
         <v>171</v>
       </c>
       <c r="H94" s="38"/>
@@ -54563,7 +54933,7 @@
         <v>205</v>
       </c>
       <c r="C95" s="25" t="s">
-        <v>31</v>
+        <v>171</v>
       </c>
       <c r="D95" s="25"/>
       <c r="E95" s="36" t="s">
@@ -54573,7 +54943,7 @@
         <v>290</v>
       </c>
       <c r="G95" s="25" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="H95" s="38"/>
       <c r="I95" s="25"/>
@@ -54597,7 +54967,7 @@
         <v>205</v>
       </c>
       <c r="C96" s="25" t="s">
-        <v>31</v>
+        <v>171</v>
       </c>
       <c r="D96" s="25"/>
       <c r="E96" s="36" t="s">
@@ -54607,7 +54977,7 @@
         <v>210</v>
       </c>
       <c r="G96" s="25" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="H96" s="38"/>
       <c r="I96" s="25"/>
@@ -54699,7 +55069,7 @@
         <v>207</v>
       </c>
       <c r="C99" s="25" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="D99" s="25"/>
       <c r="E99" s="36" t="s">
@@ -55005,7 +55375,7 @@
         <v>261</v>
       </c>
       <c r="C108" s="25" t="s">
-        <v>166</v>
+        <v>31</v>
       </c>
       <c r="D108" s="25"/>
       <c r="E108" s="25" t="s">
@@ -55389,7 +55759,7 @@
         <v>67</v>
       </c>
       <c r="G119" s="25" t="s">
-        <v>32</v>
+        <v>361</v>
       </c>
       <c r="H119" s="38"/>
       <c r="I119" s="25"/>
@@ -55645,22 +56015,158 @@
       <c r="U126" s="25"/>
       <c r="V126" s="25"/>
     </row>
+    <row r="127" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B127" s="24" t="s">
+        <v>370</v>
+      </c>
+      <c r="C127" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E127" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="F127" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="G127" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="128" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B128" s="24" t="s">
+        <v>372</v>
+      </c>
+      <c r="C128" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E128" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="F128" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="G128" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B129" s="24" t="s">
+        <v>373</v>
+      </c>
+      <c r="C129" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E129" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="F129" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="G129" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B130" s="24" t="s">
+        <v>374</v>
+      </c>
+      <c r="C130" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E130" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="F130" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="G130" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B131" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="C131" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E131" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="F131" s="25" t="s">
+        <v>381</v>
+      </c>
+      <c r="G131" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B132" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="C132" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E132" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="F132" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="G132" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B133" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="C133" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E133" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="F133" s="25" t="s">
+        <v>380</v>
+      </c>
+      <c r="G133" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B134" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="C134" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E134" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="F134" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="G134" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:V126"/>
   <sortState ref="A2:V112">
     <sortCondition ref="B2:B112"/>
   </sortState>
   <conditionalFormatting sqref="B127:B1048576 B1">
-    <cfRule type="duplicateValues" dxfId="3" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F124">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="F2:F124 F127:F134">
+    <cfRule type="duplicateValues" dxfId="32" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F125:F126">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F59">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -55674,7 +56180,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -55796,11 +56302,11 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:Z883"/>
+  <dimension ref="A1:Z939"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -63094,12 +63600,481 @@
         <v>362</v>
       </c>
     </row>
+    <row r="884" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B884" t="s">
+        <v>138</v>
+      </c>
+      <c r="D884" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="885" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B885" t="s">
+        <v>138</v>
+      </c>
+      <c r="D885" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="886" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B886" t="s">
+        <v>138</v>
+      </c>
+      <c r="D886" s="24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="887" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B887" t="s">
+        <v>138</v>
+      </c>
+      <c r="D887" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="888" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B888" t="s">
+        <v>138</v>
+      </c>
+      <c r="D888" s="24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="889" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B889" t="s">
+        <v>138</v>
+      </c>
+      <c r="D889" s="24" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="890" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B890" t="s">
+        <v>138</v>
+      </c>
+      <c r="D890" s="24" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="891" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B891" t="s">
+        <v>138</v>
+      </c>
+      <c r="D891" s="24" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="892" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B892" t="s">
+        <v>149</v>
+      </c>
+      <c r="D892" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="893" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B893" t="s">
+        <v>149</v>
+      </c>
+      <c r="D893" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="894" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B894" t="s">
+        <v>149</v>
+      </c>
+      <c r="D894" s="24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="895" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B895" t="s">
+        <v>149</v>
+      </c>
+      <c r="D895" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="896" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B896" t="s">
+        <v>149</v>
+      </c>
+      <c r="D896" s="24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="897" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B897" t="s">
+        <v>149</v>
+      </c>
+      <c r="D897" s="24" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="898" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B898" t="s">
+        <v>149</v>
+      </c>
+      <c r="D898" s="24" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="899" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B899" t="s">
+        <v>149</v>
+      </c>
+      <c r="D899" s="24" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="900" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B900" t="s">
+        <v>150</v>
+      </c>
+      <c r="D900" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="901" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B901" t="s">
+        <v>150</v>
+      </c>
+      <c r="D901" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="902" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B902" t="s">
+        <v>150</v>
+      </c>
+      <c r="D902" s="24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="903" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B903" t="s">
+        <v>150</v>
+      </c>
+      <c r="D903" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="904" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B904" t="s">
+        <v>150</v>
+      </c>
+      <c r="D904" s="24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="905" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B905" t="s">
+        <v>150</v>
+      </c>
+      <c r="D905" s="24" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="906" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B906" t="s">
+        <v>150</v>
+      </c>
+      <c r="D906" s="24" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="907" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B907" t="s">
+        <v>150</v>
+      </c>
+      <c r="D907" s="24" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="908" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B908" t="s">
+        <v>151</v>
+      </c>
+      <c r="D908" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="909" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B909" t="s">
+        <v>151</v>
+      </c>
+      <c r="D909" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="910" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B910" t="s">
+        <v>151</v>
+      </c>
+      <c r="D910" s="24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="911" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B911" t="s">
+        <v>151</v>
+      </c>
+      <c r="D911" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="912" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B912" t="s">
+        <v>151</v>
+      </c>
+      <c r="D912" s="24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="913" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B913" t="s">
+        <v>151</v>
+      </c>
+      <c r="D913" s="24" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="914" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B914" t="s">
+        <v>151</v>
+      </c>
+      <c r="D914" s="24" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="915" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B915" t="s">
+        <v>151</v>
+      </c>
+      <c r="D915" s="24" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="916" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B916" t="s">
+        <v>155</v>
+      </c>
+      <c r="D916" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="917" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B917" t="s">
+        <v>155</v>
+      </c>
+      <c r="D917" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="918" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B918" t="s">
+        <v>155</v>
+      </c>
+      <c r="D918" s="24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="919" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B919" t="s">
+        <v>155</v>
+      </c>
+      <c r="D919" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="920" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B920" t="s">
+        <v>155</v>
+      </c>
+      <c r="D920" s="24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="921" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B921" t="s">
+        <v>155</v>
+      </c>
+      <c r="D921" s="24" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="922" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B922" t="s">
+        <v>155</v>
+      </c>
+      <c r="D922" s="24" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="923" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B923" t="s">
+        <v>155</v>
+      </c>
+      <c r="D923" s="24" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="924" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B924" t="s">
+        <v>156</v>
+      </c>
+      <c r="D924" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="925" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B925" t="s">
+        <v>156</v>
+      </c>
+      <c r="D925" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="926" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B926" t="s">
+        <v>156</v>
+      </c>
+      <c r="D926" s="24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="927" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B927" t="s">
+        <v>156</v>
+      </c>
+      <c r="D927" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="928" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B928" t="s">
+        <v>156</v>
+      </c>
+      <c r="D928" s="24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="929" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B929" t="s">
+        <v>156</v>
+      </c>
+      <c r="D929" s="24" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="930" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B930" t="s">
+        <v>156</v>
+      </c>
+      <c r="D930" s="24" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="931" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B931" t="s">
+        <v>156</v>
+      </c>
+      <c r="D931" s="24" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="932" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B932" t="s">
+        <v>157</v>
+      </c>
+      <c r="D932" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="933" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B933" t="s">
+        <v>157</v>
+      </c>
+      <c r="D933" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="934" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B934" t="s">
+        <v>157</v>
+      </c>
+      <c r="D934" s="24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="935" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B935" t="s">
+        <v>157</v>
+      </c>
+      <c r="D935" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="936" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B936" t="s">
+        <v>157</v>
+      </c>
+      <c r="D936" s="24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="937" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B937" t="s">
+        <v>157</v>
+      </c>
+      <c r="D937" s="24" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="938" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B938" t="s">
+        <v>157</v>
+      </c>
+      <c r="D938" s="24" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="939" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B939" t="s">
+        <v>157</v>
+      </c>
+      <c r="D939" s="24" t="s">
+        <v>378</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:Z883"/>
   <sortState ref="A2:Y722">
     <sortCondition ref="B2:B722"/>
     <sortCondition ref="D2:D722"/>
   </sortState>
+  <conditionalFormatting sqref="D884:D891">
+    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D892:D899">
+    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D900:D907">
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D908:D915">
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D916:D923">
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D924:D931">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D932:D939">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>